<commit_message>
use QLXL template workbook for HKD
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/Book1.xlsx
+++ b/QuantLibXL/Data2/Book1.xlsx
@@ -7,25 +7,51 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="17235" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="HKD" sheetId="4" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="qlxlProgramColumns" localSheetId="0">HKD!$A:$E</definedName>
+    <definedName name="qlxlProgramRows" localSheetId="0">HKD!$1:$10</definedName>
+    <definedName name="qlxlWorksheetType" localSheetId="0">""</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
-    <t>Fixed Income 2</t>
+    <t>Object Group</t>
+  </si>
+  <si>
+    <t>Header 2</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Data Read/Write</t>
+  </si>
+  <si>
+    <t>Data ReadOnly</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Object Scalar</t>
+  </si>
+  <si>
+    <t>HKD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,16 +59,112 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3" tint="0.39994506668294322"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFCC"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59996337778862885"/>
+        <bgColor theme="3" tint="0.59996337778862885"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor theme="3" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -50,15 +172,192 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="8" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="9" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="8" xfId="10" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="8" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="qlxlBackround" xfId="2"/>
+    <cellStyle name="qlxlDataReadOnly" xfId="8"/>
+    <cellStyle name="qlxlDataReadWrite" xfId="7"/>
+    <cellStyle name="qlxlHeader1" xfId="3"/>
+    <cellStyle name="qlxlHeader2" xfId="5"/>
+    <cellStyle name="qlxlLabel" xfId="6"/>
+    <cellStyle name="qlxlObjectGroup" xfId="4"/>
+    <cellStyle name="qlxlObjectScalar" xfId="10"/>
+    <cellStyle name="qlxlStatus" xfId="9"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -358,21 +657,428 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F11" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="5" width="9.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2"/>
+    <col min="7" max="7" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="256" width="9.140625" style="2"/>
+    <col min="257" max="261" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="262" max="262" width="9.140625" style="2"/>
+    <col min="263" max="263" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="265" max="512" width="9.140625" style="2"/>
+    <col min="513" max="517" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="518" max="518" width="9.140625" style="2"/>
+    <col min="519" max="519" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="520" max="520" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="521" max="768" width="9.140625" style="2"/>
+    <col min="769" max="773" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="774" max="774" width="9.140625" style="2"/>
+    <col min="775" max="775" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="776" max="776" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="777" max="1024" width="9.140625" style="2"/>
+    <col min="1025" max="1029" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="1030" max="1030" width="9.140625" style="2"/>
+    <col min="1031" max="1031" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1032" max="1032" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1033" max="1280" width="9.140625" style="2"/>
+    <col min="1281" max="1285" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="1286" max="1286" width="9.140625" style="2"/>
+    <col min="1287" max="1287" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1288" max="1288" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1289" max="1536" width="9.140625" style="2"/>
+    <col min="1537" max="1541" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="1542" max="1542" width="9.140625" style="2"/>
+    <col min="1543" max="1543" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1544" max="1544" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1545" max="1792" width="9.140625" style="2"/>
+    <col min="1793" max="1797" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="1798" max="1798" width="9.140625" style="2"/>
+    <col min="1799" max="1799" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1800" max="1800" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1801" max="2048" width="9.140625" style="2"/>
+    <col min="2049" max="2053" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="2054" max="2054" width="9.140625" style="2"/>
+    <col min="2055" max="2055" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2056" max="2056" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2057" max="2304" width="9.140625" style="2"/>
+    <col min="2305" max="2309" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="2310" max="2310" width="9.140625" style="2"/>
+    <col min="2311" max="2311" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2312" max="2312" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2313" max="2560" width="9.140625" style="2"/>
+    <col min="2561" max="2565" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="2566" max="2566" width="9.140625" style="2"/>
+    <col min="2567" max="2567" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2568" max="2568" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2569" max="2816" width="9.140625" style="2"/>
+    <col min="2817" max="2821" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="2822" max="2822" width="9.140625" style="2"/>
+    <col min="2823" max="2823" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2824" max="2824" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2825" max="3072" width="9.140625" style="2"/>
+    <col min="3073" max="3077" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="3078" max="3078" width="9.140625" style="2"/>
+    <col min="3079" max="3079" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3080" max="3080" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3081" max="3328" width="9.140625" style="2"/>
+    <col min="3329" max="3333" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="3334" max="3334" width="9.140625" style="2"/>
+    <col min="3335" max="3335" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3336" max="3336" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3337" max="3584" width="9.140625" style="2"/>
+    <col min="3585" max="3589" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="3590" max="3590" width="9.140625" style="2"/>
+    <col min="3591" max="3591" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3592" max="3592" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3593" max="3840" width="9.140625" style="2"/>
+    <col min="3841" max="3845" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="3846" max="3846" width="9.140625" style="2"/>
+    <col min="3847" max="3847" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3848" max="3848" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3849" max="4096" width="9.140625" style="2"/>
+    <col min="4097" max="4101" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="4102" max="4102" width="9.140625" style="2"/>
+    <col min="4103" max="4103" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4104" max="4104" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4105" max="4352" width="9.140625" style="2"/>
+    <col min="4353" max="4357" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="4358" max="4358" width="9.140625" style="2"/>
+    <col min="4359" max="4359" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4360" max="4360" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4361" max="4608" width="9.140625" style="2"/>
+    <col min="4609" max="4613" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="4614" max="4614" width="9.140625" style="2"/>
+    <col min="4615" max="4615" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4616" max="4616" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4617" max="4864" width="9.140625" style="2"/>
+    <col min="4865" max="4869" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="4870" max="4870" width="9.140625" style="2"/>
+    <col min="4871" max="4871" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4872" max="4872" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4873" max="5120" width="9.140625" style="2"/>
+    <col min="5121" max="5125" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="5126" max="5126" width="9.140625" style="2"/>
+    <col min="5127" max="5127" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5128" max="5128" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5129" max="5376" width="9.140625" style="2"/>
+    <col min="5377" max="5381" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="5382" max="5382" width="9.140625" style="2"/>
+    <col min="5383" max="5383" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5384" max="5384" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5385" max="5632" width="9.140625" style="2"/>
+    <col min="5633" max="5637" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="5638" max="5638" width="9.140625" style="2"/>
+    <col min="5639" max="5639" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5640" max="5640" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5641" max="5888" width="9.140625" style="2"/>
+    <col min="5889" max="5893" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="5894" max="5894" width="9.140625" style="2"/>
+    <col min="5895" max="5895" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5896" max="5896" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5897" max="6144" width="9.140625" style="2"/>
+    <col min="6145" max="6149" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="6150" max="6150" width="9.140625" style="2"/>
+    <col min="6151" max="6151" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6152" max="6152" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6153" max="6400" width="9.140625" style="2"/>
+    <col min="6401" max="6405" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="6406" max="6406" width="9.140625" style="2"/>
+    <col min="6407" max="6407" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6408" max="6408" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6409" max="6656" width="9.140625" style="2"/>
+    <col min="6657" max="6661" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="6662" max="6662" width="9.140625" style="2"/>
+    <col min="6663" max="6663" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6664" max="6664" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6665" max="6912" width="9.140625" style="2"/>
+    <col min="6913" max="6917" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="6918" max="6918" width="9.140625" style="2"/>
+    <col min="6919" max="6919" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6920" max="6920" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6921" max="7168" width="9.140625" style="2"/>
+    <col min="7169" max="7173" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="7174" max="7174" width="9.140625" style="2"/>
+    <col min="7175" max="7175" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7176" max="7176" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7177" max="7424" width="9.140625" style="2"/>
+    <col min="7425" max="7429" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="7430" max="7430" width="9.140625" style="2"/>
+    <col min="7431" max="7431" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7432" max="7432" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7433" max="7680" width="9.140625" style="2"/>
+    <col min="7681" max="7685" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="7686" max="7686" width="9.140625" style="2"/>
+    <col min="7687" max="7687" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7688" max="7688" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7689" max="7936" width="9.140625" style="2"/>
+    <col min="7937" max="7941" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="7942" max="7942" width="9.140625" style="2"/>
+    <col min="7943" max="7943" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7944" max="7944" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7945" max="8192" width="9.140625" style="2"/>
+    <col min="8193" max="8197" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="8198" max="8198" width="9.140625" style="2"/>
+    <col min="8199" max="8199" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8200" max="8200" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8201" max="8448" width="9.140625" style="2"/>
+    <col min="8449" max="8453" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="8454" max="8454" width="9.140625" style="2"/>
+    <col min="8455" max="8455" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8456" max="8456" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8457" max="8704" width="9.140625" style="2"/>
+    <col min="8705" max="8709" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="8710" max="8710" width="9.140625" style="2"/>
+    <col min="8711" max="8711" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8712" max="8712" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8713" max="8960" width="9.140625" style="2"/>
+    <col min="8961" max="8965" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="8966" max="8966" width="9.140625" style="2"/>
+    <col min="8967" max="8967" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8968" max="8968" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8969" max="9216" width="9.140625" style="2"/>
+    <col min="9217" max="9221" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="9222" max="9222" width="9.140625" style="2"/>
+    <col min="9223" max="9223" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9224" max="9224" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9225" max="9472" width="9.140625" style="2"/>
+    <col min="9473" max="9477" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="9478" max="9478" width="9.140625" style="2"/>
+    <col min="9479" max="9479" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9480" max="9480" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9481" max="9728" width="9.140625" style="2"/>
+    <col min="9729" max="9733" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="9734" max="9734" width="9.140625" style="2"/>
+    <col min="9735" max="9735" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9736" max="9736" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9737" max="9984" width="9.140625" style="2"/>
+    <col min="9985" max="9989" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="9990" max="9990" width="9.140625" style="2"/>
+    <col min="9991" max="9991" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9992" max="9992" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9993" max="10240" width="9.140625" style="2"/>
+    <col min="10241" max="10245" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="10246" max="10246" width="9.140625" style="2"/>
+    <col min="10247" max="10247" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10248" max="10248" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10249" max="10496" width="9.140625" style="2"/>
+    <col min="10497" max="10501" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="10502" max="10502" width="9.140625" style="2"/>
+    <col min="10503" max="10503" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10504" max="10504" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10505" max="10752" width="9.140625" style="2"/>
+    <col min="10753" max="10757" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="10758" max="10758" width="9.140625" style="2"/>
+    <col min="10759" max="10759" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10760" max="10760" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10761" max="11008" width="9.140625" style="2"/>
+    <col min="11009" max="11013" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="11014" max="11014" width="9.140625" style="2"/>
+    <col min="11015" max="11015" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11016" max="11016" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11017" max="11264" width="9.140625" style="2"/>
+    <col min="11265" max="11269" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="11270" max="11270" width="9.140625" style="2"/>
+    <col min="11271" max="11271" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11272" max="11272" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11273" max="11520" width="9.140625" style="2"/>
+    <col min="11521" max="11525" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="11526" max="11526" width="9.140625" style="2"/>
+    <col min="11527" max="11527" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11528" max="11528" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11529" max="11776" width="9.140625" style="2"/>
+    <col min="11777" max="11781" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="11782" max="11782" width="9.140625" style="2"/>
+    <col min="11783" max="11783" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11784" max="11784" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11785" max="12032" width="9.140625" style="2"/>
+    <col min="12033" max="12037" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="12038" max="12038" width="9.140625" style="2"/>
+    <col min="12039" max="12039" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12040" max="12040" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12041" max="12288" width="9.140625" style="2"/>
+    <col min="12289" max="12293" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="12294" max="12294" width="9.140625" style="2"/>
+    <col min="12295" max="12295" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12296" max="12296" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12297" max="12544" width="9.140625" style="2"/>
+    <col min="12545" max="12549" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="12550" max="12550" width="9.140625" style="2"/>
+    <col min="12551" max="12551" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12552" max="12552" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12553" max="12800" width="9.140625" style="2"/>
+    <col min="12801" max="12805" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="12806" max="12806" width="9.140625" style="2"/>
+    <col min="12807" max="12807" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12808" max="12808" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12809" max="13056" width="9.140625" style="2"/>
+    <col min="13057" max="13061" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="13062" max="13062" width="9.140625" style="2"/>
+    <col min="13063" max="13063" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13064" max="13064" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13065" max="13312" width="9.140625" style="2"/>
+    <col min="13313" max="13317" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="13318" max="13318" width="9.140625" style="2"/>
+    <col min="13319" max="13319" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13320" max="13320" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13321" max="13568" width="9.140625" style="2"/>
+    <col min="13569" max="13573" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="13574" max="13574" width="9.140625" style="2"/>
+    <col min="13575" max="13575" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13576" max="13576" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13577" max="13824" width="9.140625" style="2"/>
+    <col min="13825" max="13829" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="13830" max="13830" width="9.140625" style="2"/>
+    <col min="13831" max="13831" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13832" max="13832" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13833" max="14080" width="9.140625" style="2"/>
+    <col min="14081" max="14085" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="14086" max="14086" width="9.140625" style="2"/>
+    <col min="14087" max="14087" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14088" max="14088" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14089" max="14336" width="9.140625" style="2"/>
+    <col min="14337" max="14341" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="14342" max="14342" width="9.140625" style="2"/>
+    <col min="14343" max="14343" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14344" max="14344" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14345" max="14592" width="9.140625" style="2"/>
+    <col min="14593" max="14597" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="14598" max="14598" width="9.140625" style="2"/>
+    <col min="14599" max="14599" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14600" max="14600" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14601" max="14848" width="9.140625" style="2"/>
+    <col min="14849" max="14853" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="14854" max="14854" width="9.140625" style="2"/>
+    <col min="14855" max="14855" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14856" max="14856" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14857" max="15104" width="9.140625" style="2"/>
+    <col min="15105" max="15109" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="15110" max="15110" width="9.140625" style="2"/>
+    <col min="15111" max="15111" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15112" max="15112" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15113" max="15360" width="9.140625" style="2"/>
+    <col min="15361" max="15365" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="15366" max="15366" width="9.140625" style="2"/>
+    <col min="15367" max="15367" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15368" max="15368" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15369" max="15616" width="9.140625" style="2"/>
+    <col min="15617" max="15621" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="15622" max="15622" width="9.140625" style="2"/>
+    <col min="15623" max="15623" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15624" max="15624" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15625" max="15872" width="9.140625" style="2"/>
+    <col min="15873" max="15877" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="15878" max="15878" width="9.140625" style="2"/>
+    <col min="15879" max="15879" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15880" max="15880" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15881" max="16128" width="9.140625" style="2"/>
+    <col min="16129" max="16133" width="0" style="2" hidden="1" customWidth="1"/>
+    <col min="16134" max="16134" width="9.140625" style="2"/>
+    <col min="16135" max="16135" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16136" max="16136" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16137" max="16384" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="7:9" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="7:9" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="7:9" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="7:9" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="7:9" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="7:9" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="7:9" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="7:9" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="7:9" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="7:9" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="7:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="7:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="7:9" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="7:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="7" t="s">
         <v>0</v>
+      </c>
+      <c r="H14" s="8"/>
+    </row>
+    <row r="15" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G15" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="7:9" x14ac:dyDescent="0.2">
+      <c r="G16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G17" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G18" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G19" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G20" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="7:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <mergeCells count="2">
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G14:H14"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 

</xml_diff>